<commit_message>
Postman deployment set up
</commit_message>
<xml_diff>
--- a/OPCIONES MODELOS.xlsx
+++ b/OPCIONES MODELOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\UNIVERSIDAD\1 SEMESTRE\CIENCIA DE DATOS APLICADA\TALLER 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Maestria\2023-20\CIENCIA DE DATOS APLICADA\Talleres\03 - Model Serving\MINE4101-T3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{964B627D-7985-4CCB-95E2-28308C1FFF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A200D1-967C-4161-8FFA-147EFD36686F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8700CC9-FFD9-4535-99BA-85F90EEFF41E}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{E8700CC9-FFD9-4535-99BA-85F90EEFF41E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,15 +467,16 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="68.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -486,7 +487,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -497,7 +498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -508,7 +509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -519,7 +520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -530,7 +531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -541,7 +542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -552,7 +553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -563,7 +564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -574,7 +575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -585,7 +586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -596,7 +597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -607,7 +608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -618,7 +619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
     </row>
   </sheetData>

</xml_diff>